<commit_message>
update link tesst + default account
</commit_message>
<xml_diff>
--- a/testing/dataSheet.xlsx
+++ b/testing/dataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\SoftwareTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\doctor_assignment_BE\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D538120-B0C1-49D9-B0F6-4E1F70BA382B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667E1FEE-AA37-4263-ABE1-97EFE8C4C225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTC1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="72">
   <si>
     <t>username</t>
   </si>
@@ -205,9 +205,6 @@
   </si>
   <si>
     <t>Please select your date of birth!</t>
-  </si>
-  <si>
-    <t>'0123456790</t>
   </si>
   <si>
     <t>aaaaabbzbb@gmail.com</t>
@@ -598,7 +595,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +622,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -706,16 +703,16 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
       </c>
       <c r="H2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -738,10 +735,10 @@
         <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -817,16 +814,16 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
       </c>
       <c r="H2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" t="s">
         <v>59</v>
-      </c>
-      <c r="I2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -849,10 +846,10 @@
         <v>47</v>
       </c>
       <c r="H3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" t="s">
         <v>59</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -929,16 +926,16 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
         <v>47</v>
       </c>
       <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
         <v>61</v>
-      </c>
-      <c r="I2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -962,10 +959,10 @@
         <v>47</v>
       </c>
       <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" t="s">
         <v>61</v>
-      </c>
-      <c r="I3" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1044,13 +1041,13 @@
         <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1073,10 +1070,10 @@
         <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1105,10 +1102,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -1125,10 +1122,10 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>67</v>
-      </c>
-      <c r="D2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1154,10 +1151,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -1171,10 +1168,10 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1184,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FD0457-BECA-471C-B45D-E4486972E038}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1200,10 +1197,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -1218,10 +1215,10 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
         <v>71</v>
-      </c>
-      <c r="D2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1234,7 +1231,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,7 +1258,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>123</v>
@@ -1275,7 +1272,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>456</v>
@@ -1494,7 +1491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D4ECCE-691F-46BB-8B31-BB1C5C175842}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>

</xml_diff>